<commit_message>
Remove old excel files
</commit_message>
<xml_diff>
--- a/towns.xlsx
+++ b/towns.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zissou/IdeaProjects/College/YearTwo/SemesterTwo/app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zissou/Library/Mobile Documents/com~apple~CloudDocs/College/YearTwo/SemesterTwo/DSII/code/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926A84F8-4D14-B341-AE90-D1AF619B816C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7740442-7BAE-3847-9C8C-F4A8213E6B37}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="460" windowWidth="26680" windowHeight="13920" xr2:uid="{DBCE131A-A3CE-4E2D-AF18-B48AB3E1F46A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" activeTab="1" xr2:uid="{DBCE131A-A3CE-4E2D-AF18-B48AB3E1F46A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Nodes" sheetId="1" r:id="rId1"/>
+    <sheet name="Edges" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,6 +58,9 @@
     <t>Ar Noy</t>
   </si>
   <si>
+    <t>The Sorows</t>
+  </si>
+  <si>
     <t>Myr</t>
   </si>
   <si>
@@ -212,9 +215,6 @@
   </si>
   <si>
     <t>Sunspear</t>
-  </si>
-  <si>
-    <t>The Sorrows</t>
   </si>
 </sst>
 </file>
@@ -574,10 +574,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D590995-89BF-4F4C-BA1D-DA71ED025EC1}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T146"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:D61"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -592,7 +593,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C1">
         <v>965</v>
@@ -606,7 +607,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2">
         <v>1026</v>
@@ -620,7 +621,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3">
         <v>823</v>
@@ -634,7 +635,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C4">
         <v>669</v>
@@ -648,7 +649,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C5">
         <v>927</v>
@@ -662,7 +663,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C6">
         <v>822</v>
@@ -676,7 +677,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C7">
         <v>798</v>
@@ -690,7 +691,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C8">
         <v>1036</v>
@@ -704,7 +705,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C9">
         <v>1211</v>
@@ -718,7 +719,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C10">
         <v>910</v>
@@ -732,7 +733,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C11">
         <v>754</v>
@@ -746,7 +747,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C12">
         <v>526</v>
@@ -760,7 +761,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C13">
         <v>555</v>
@@ -774,7 +775,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C14">
         <v>499</v>
@@ -788,7 +789,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C15">
         <v>516</v>
@@ -802,10 +803,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C16">
-        <v>516</v>
+        <v>561</v>
       </c>
       <c r="D16">
         <v>1645</v>
@@ -816,7 +817,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C17">
         <v>1172</v>
@@ -830,7 +831,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C18">
         <v>979</v>
@@ -845,7 +846,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C19">
         <v>1125</v>
@@ -859,7 +860,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C20">
         <v>630</v>
@@ -873,7 +874,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C21">
         <v>516</v>
@@ -887,7 +888,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C22">
         <v>1204</v>
@@ -1013,7 +1014,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="C31">
         <v>1796</v>
@@ -1027,7 +1028,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C32">
         <v>1555</v>
@@ -1041,7 +1042,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C33">
         <v>1348</v>
@@ -1055,7 +1056,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C34">
         <v>1829</v>
@@ -1069,7 +1070,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C35">
         <v>1817</v>
@@ -1083,7 +1084,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C36">
         <v>1472</v>
@@ -1097,7 +1098,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C37">
         <v>1843</v>
@@ -1111,7 +1112,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C38">
         <v>1860</v>
@@ -1125,7 +1126,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C39">
         <v>1914</v>
@@ -1139,7 +1140,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C40">
         <v>2250</v>
@@ -1153,7 +1154,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C41">
         <v>2222</v>
@@ -1167,7 +1168,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C42">
         <v>2198</v>
@@ -1181,7 +1182,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C43">
         <v>2160</v>
@@ -1195,7 +1196,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C44">
         <v>2360</v>
@@ -1209,7 +1210,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C45">
         <v>2488</v>
@@ -1223,7 +1224,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C46">
         <v>2710</v>
@@ -1237,7 +1238,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C47">
         <v>2641</v>
@@ -1251,7 +1252,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C48">
         <v>2606</v>
@@ -1265,7 +1266,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C49">
         <v>2426</v>
@@ -1279,7 +1280,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C50">
         <v>2441</v>
@@ -1293,7 +1294,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C51">
         <v>2643</v>
@@ -1307,7 +1308,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C52">
         <v>2680</v>
@@ -1321,7 +1322,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C53">
         <v>2240</v>
@@ -1335,7 +1336,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C54">
         <v>2184</v>
@@ -1349,7 +1350,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C55">
         <v>2323</v>
@@ -1363,7 +1364,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C56">
         <v>2373</v>
@@ -1377,7 +1378,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C57">
         <v>2460</v>
@@ -1391,7 +1392,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C58">
         <v>2615</v>
@@ -1405,7 +1406,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C59">
         <v>2742</v>
@@ -1419,7 +1420,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C60">
         <v>2670</v>
@@ -1433,7 +1434,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C61">
         <v>2724</v>
@@ -1458,167 +1459,168 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B6A9F9A-B06F-0741-97AC-5B838BA1D1A9}">
-  <dimension ref="A1:D124"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DA4984-602A-D449-B363-ADE69DAEFD28}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:D161"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="F122" sqref="F122"/>
+    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="D161" sqref="D161"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>2</v>
-      </c>
       <c r="C1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D1">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
       <c r="C3">
-        <v>2</v>
+        <v>83</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>57</v>
+      </c>
+      <c r="D4">
         <v>2</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
         <v>2</v>
       </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
       <c r="C5">
-        <v>3</v>
+        <v>86</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
         <v>2</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
       <c r="C6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="D8">
-        <v>8</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B9">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C9">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="D9">
-        <v>6</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1629,66 +1631,66 @@
         <v>4</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>93</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B13">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C13">
         <v>3</v>
       </c>
       <c r="D13">
-        <v>4</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B14">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>67</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B15">
         <v>5</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C16">
-        <v>6</v>
+        <v>90</v>
       </c>
       <c r="D16">
-        <v>7</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1699,38 +1701,38 @@
         <v>6</v>
       </c>
       <c r="C17">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="D17">
-        <v>9</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B18">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B19">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1741,10 +1743,10 @@
         <v>7</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1752,262 +1754,262 @@
         <v>9</v>
       </c>
       <c r="B21">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D21">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B22">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D22">
-        <v>7</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B23">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>98</v>
       </c>
       <c r="D23">
-        <v>8</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B25">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="D25">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B26">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C26">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="D26">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B27">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="D27">
-        <v>3</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B28">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C28">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B29">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="D29">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B30">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B31">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C31">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="D31">
-        <v>4</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B32">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C32">
-        <v>7</v>
+        <v>78</v>
       </c>
       <c r="D32">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B33">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B34">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C34">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D34">
-        <v>10</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>16</v>
-      </c>
-      <c r="B35" s="1">
-        <v>26</v>
-      </c>
-      <c r="C35" s="1">
-        <v>5</v>
-      </c>
-      <c r="D35" s="1">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="B35">
+        <v>11</v>
+      </c>
+      <c r="C35">
+        <v>28</v>
+      </c>
+      <c r="D35">
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>16</v>
-      </c>
-      <c r="B36" s="1">
-        <v>32</v>
-      </c>
-      <c r="C36" s="1">
-        <v>6</v>
-      </c>
-      <c r="D36" s="1">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="B36">
+        <v>11</v>
+      </c>
+      <c r="C36">
+        <v>38</v>
+      </c>
+      <c r="D36">
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B37">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C37">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="D37">
-        <v>7</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B38">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C38">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="D38">
-        <v>6</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B39">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="D39">
         <v>4</v>
@@ -2015,1197 +2017,1715 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B40">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C40">
-        <v>3</v>
+        <v>90</v>
       </c>
       <c r="D40">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B41">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C41">
-        <v>7</v>
+        <v>92</v>
       </c>
       <c r="D41">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B42">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C42">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="D42">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B43">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C43">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B44">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="C44">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D44">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B45">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>87</v>
       </c>
       <c r="D45">
-        <v>4</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B46">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C46">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="D46">
-        <v>3</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B47">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C47">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D47">
-        <v>3</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B48">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="C48">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="D48">
-        <v>3</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B49">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C49">
-        <v>3</v>
+        <v>96</v>
       </c>
       <c r="D49">
-        <v>2</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>24</v>
+      <c r="A50" s="1">
+        <v>26</v>
       </c>
       <c r="B50">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C50">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D50">
-        <v>6</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>25</v>
+      <c r="A51" s="1">
+        <v>32</v>
       </c>
       <c r="B51">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D51">
-        <v>2</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B52">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C52">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="D52">
-        <v>3</v>
+        <v>84</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B53">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C53">
-        <v>2</v>
+        <v>91</v>
       </c>
       <c r="D53">
-        <v>4</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B54">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C54">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D54">
-        <v>3</v>
+        <v>68</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B55">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="D55">
-        <v>1</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B56">
+        <v>18</v>
+      </c>
+      <c r="C56">
         <v>27</v>
       </c>
-      <c r="C56">
-        <v>3</v>
-      </c>
       <c r="D56">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B57">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C57">
-        <v>3</v>
+        <v>82</v>
       </c>
       <c r="D57">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B58">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C58">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="D58">
-        <v>1</v>
+        <v>70</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B59">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C59">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D59">
-        <v>2</v>
+        <v>67</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B60">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>44</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B61">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C61">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="D61">
-        <v>3</v>
+        <v>96</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B62">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="D62">
-        <v>2</v>
+        <v>55</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B63">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="C63">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D63">
-        <v>4</v>
+        <v>94</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B64">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="C64">
-        <v>4</v>
+        <v>94</v>
       </c>
       <c r="D64">
-        <v>8</v>
+        <v>43</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="B65">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C65">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="D65">
-        <v>2</v>
+        <v>27</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B66">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C66">
-        <v>2</v>
+        <v>88</v>
       </c>
       <c r="D66">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B67">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C67">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="D67">
-        <v>3</v>
+        <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B68">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C68">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="D68">
-        <v>2</v>
+        <v>77</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="B69">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C69">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="D69">
-        <v>3</v>
+        <v>64</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B70">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C70">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D70">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="B71">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C71">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="D71">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72">
+        <v>25</v>
+      </c>
+      <c r="B72">
+        <v>24</v>
+      </c>
+      <c r="C72">
+        <v>82</v>
+      </c>
+      <c r="D72">
         <v>35</v>
-      </c>
-      <c r="B72">
-        <v>21</v>
-      </c>
-      <c r="C72">
-        <v>3</v>
-      </c>
-      <c r="D72">
-        <v>3</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B73">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C73">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="D73">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B74">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C74">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="D74">
-        <v>2</v>
+        <v>40</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B75">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C75">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="D75">
-        <v>1</v>
+        <v>82</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="B76">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C76">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="D76">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>38</v>
-      </c>
-      <c r="B77">
-        <v>51</v>
+        <v>16</v>
+      </c>
+      <c r="B77" s="1">
+        <v>26</v>
       </c>
       <c r="C77">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D77">
-        <v>9</v>
+        <v>33</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B78">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C78">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="D78">
-        <v>4</v>
+        <v>89</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B79">
+        <v>26</v>
+      </c>
+      <c r="C79">
         <v>37</v>
       </c>
-      <c r="C79">
-        <v>2</v>
-      </c>
       <c r="D79">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B80">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C80">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D80">
-        <v>3</v>
+        <v>46</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B81">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="C81">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="D81">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B82">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C82">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="D82">
-        <v>5</v>
+        <v>83</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B83">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C83">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="D83">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B84">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="C84">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D84">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B85">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="C85">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="D85">
-        <v>8</v>
+        <v>37</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B86">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="C86">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="D86">
-        <v>8</v>
+        <v>57</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B87">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C87">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="D87">
-        <v>6</v>
+        <v>96</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="B88">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C88">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="D88">
-        <v>10</v>
+        <v>74</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B89">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="C89">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D89">
-        <v>7</v>
+        <v>85</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B90">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C90">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="D90">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B91">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C91">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="D91">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B92">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C92">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D92">
-        <v>4</v>
+        <v>77</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>44</v>
-      </c>
-      <c r="B93">
-        <v>47</v>
+        <v>16</v>
+      </c>
+      <c r="B93" s="1">
+        <v>32</v>
       </c>
       <c r="C93">
-        <v>3</v>
+        <v>88</v>
       </c>
       <c r="D93">
-        <v>6</v>
+        <v>79</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B94">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C94">
-        <v>3</v>
+        <v>92</v>
       </c>
       <c r="D94">
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B95">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C95">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="D95">
-        <v>8</v>
+        <v>68</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B96">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C96">
-        <v>3</v>
+        <v>86</v>
       </c>
       <c r="D96">
-        <v>2</v>
+        <v>95</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="B97">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="C97">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D97">
-        <v>4</v>
+        <v>46</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B98">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C98">
-        <v>3</v>
+        <v>82</v>
       </c>
       <c r="D98">
-        <v>2</v>
+        <v>33</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B99">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C99">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D99">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B100">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C100">
-        <v>8</v>
+        <v>91</v>
       </c>
       <c r="D100">
-        <v>8</v>
+        <v>88</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B101">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C101">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="D101">
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B102">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="C102">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="D102">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B103">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C103">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D103">
-        <v>2</v>
+        <v>95</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B104">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C104">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="D104">
-        <v>5</v>
+        <v>90</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B105">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C105">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="D105">
-        <v>3</v>
+        <v>68</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B106">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C106">
-        <v>3</v>
+        <v>58</v>
       </c>
       <c r="D106">
-        <v>3</v>
+        <v>25</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B107">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="C107">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D107">
-        <v>2</v>
+        <v>92</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B108">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C108">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="D108">
-        <v>2</v>
+        <v>35</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B109">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="C109">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="D109">
-        <v>3</v>
+        <v>86</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B110">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C110">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="D110">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B111">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C111">
-        <v>5</v>
+        <v>79</v>
       </c>
       <c r="D111">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B112">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C112">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="D112">
-        <v>4</v>
+        <v>53</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B113">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C113">
-        <v>2</v>
+        <v>93</v>
       </c>
       <c r="D113">
-        <v>1</v>
+        <v>84</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B114">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="C114">
-        <v>4</v>
+        <v>82</v>
       </c>
       <c r="D114">
-        <v>3</v>
+        <v>71</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B115">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C115">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D115">
-        <v>3</v>
+        <v>67</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B116">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C116">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="D116">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B117">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C117">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="D117">
-        <v>3</v>
+        <v>58</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B118">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="C118">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="D118">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B119">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C119">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="D119">
-        <v>2</v>
+        <v>89</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="B120">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C120">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D120">
-        <v>2</v>
+        <v>45</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B121">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C121">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="D121">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B122">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C122">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D122">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B123">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C123">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="D123">
-        <v>2</v>
+        <v>51</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="B124">
+        <v>44</v>
+      </c>
+      <c r="C124">
+        <v>6</v>
+      </c>
+      <c r="D124">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>46</v>
+      </c>
+      <c r="B125">
+        <v>45</v>
+      </c>
+      <c r="C125">
+        <v>59</v>
+      </c>
+      <c r="D125">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>43</v>
+      </c>
+      <c r="B126">
+        <v>46</v>
+      </c>
+      <c r="C126">
+        <v>56</v>
+      </c>
+      <c r="D126">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>44</v>
+      </c>
+      <c r="B127">
+        <v>46</v>
+      </c>
+      <c r="C127">
+        <v>84</v>
+      </c>
+      <c r="D127">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>47</v>
+      </c>
+      <c r="B128">
+        <v>46</v>
+      </c>
+      <c r="C128">
+        <v>83</v>
+      </c>
+      <c r="D128">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>43</v>
+      </c>
+      <c r="B129">
+        <v>47</v>
+      </c>
+      <c r="C129">
+        <v>62</v>
+      </c>
+      <c r="D129">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>44</v>
+      </c>
+      <c r="B130">
+        <v>47</v>
+      </c>
+      <c r="C130">
+        <v>78</v>
+      </c>
+      <c r="D130">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>48</v>
+      </c>
+      <c r="B131">
+        <v>47</v>
+      </c>
+      <c r="C131">
+        <v>54</v>
+      </c>
+      <c r="D131">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>50</v>
+      </c>
+      <c r="B132">
+        <v>47</v>
+      </c>
+      <c r="C132">
+        <v>90</v>
+      </c>
+      <c r="D132">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>43</v>
+      </c>
+      <c r="B133">
+        <v>48</v>
+      </c>
+      <c r="C133">
+        <v>16</v>
+      </c>
+      <c r="D133">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>44</v>
+      </c>
+      <c r="B134">
+        <v>48</v>
+      </c>
+      <c r="C134">
+        <v>93</v>
+      </c>
+      <c r="D134">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>47</v>
+      </c>
+      <c r="B135">
+        <v>48</v>
+      </c>
+      <c r="C135">
+        <v>100</v>
+      </c>
+      <c r="D135">
         <v>26</v>
       </c>
-      <c r="C124">
-        <v>4</v>
-      </c>
-      <c r="D124">
-        <v>3</v>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>49</v>
+      </c>
+      <c r="B136">
+        <v>48</v>
+      </c>
+      <c r="C136">
+        <v>88</v>
+      </c>
+      <c r="D136">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>50</v>
+      </c>
+      <c r="B137">
+        <v>48</v>
+      </c>
+      <c r="C137">
+        <v>81</v>
+      </c>
+      <c r="D137">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>50</v>
+      </c>
+      <c r="B138">
+        <v>49</v>
+      </c>
+      <c r="C138">
+        <v>68</v>
+      </c>
+      <c r="D138">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>51</v>
+      </c>
+      <c r="B139">
+        <v>49</v>
+      </c>
+      <c r="C139">
+        <v>100</v>
+      </c>
+      <c r="D139">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>41</v>
+      </c>
+      <c r="B140">
+        <v>50</v>
+      </c>
+      <c r="C140">
+        <v>60</v>
+      </c>
+      <c r="D140">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>48</v>
+      </c>
+      <c r="B141">
+        <v>50</v>
+      </c>
+      <c r="C141">
+        <v>75</v>
+      </c>
+      <c r="D141">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>51</v>
+      </c>
+      <c r="B142">
+        <v>50</v>
+      </c>
+      <c r="C142">
+        <v>65</v>
+      </c>
+      <c r="D142">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>38</v>
+      </c>
+      <c r="B143">
+        <v>51</v>
+      </c>
+      <c r="C143">
+        <v>27</v>
+      </c>
+      <c r="D143">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>41</v>
+      </c>
+      <c r="B144">
+        <v>51</v>
+      </c>
+      <c r="C144">
+        <v>99</v>
+      </c>
+      <c r="D144">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>41</v>
+      </c>
+      <c r="B145">
+        <v>51</v>
+      </c>
+      <c r="C145">
+        <v>73</v>
+      </c>
+      <c r="D145">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>49</v>
+      </c>
+      <c r="B146">
+        <v>51</v>
+      </c>
+      <c r="C146">
+        <v>42</v>
+      </c>
+      <c r="D146">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>53</v>
+      </c>
+      <c r="B147">
+        <v>52</v>
+      </c>
+      <c r="C147">
+        <v>33</v>
+      </c>
+      <c r="D147">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>54</v>
+      </c>
+      <c r="B148">
+        <v>52</v>
+      </c>
+      <c r="C148">
+        <v>82</v>
+      </c>
+      <c r="D148">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>55</v>
+      </c>
+      <c r="B149">
+        <v>52</v>
+      </c>
+      <c r="C149">
+        <v>12</v>
+      </c>
+      <c r="D149">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>22</v>
+      </c>
+      <c r="B150">
+        <v>53</v>
+      </c>
+      <c r="C150">
+        <v>94</v>
+      </c>
+      <c r="D150">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>56</v>
+      </c>
+      <c r="B151">
+        <v>53</v>
+      </c>
+      <c r="C151">
+        <v>13</v>
+      </c>
+      <c r="D151">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>23</v>
+      </c>
+      <c r="B152">
+        <v>54</v>
+      </c>
+      <c r="C152">
+        <v>33</v>
+      </c>
+      <c r="D152">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>52</v>
+      </c>
+      <c r="B153">
+        <v>54</v>
+      </c>
+      <c r="C153">
+        <v>82</v>
+      </c>
+      <c r="D153">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>55</v>
+      </c>
+      <c r="B154">
+        <v>54</v>
+      </c>
+      <c r="C154">
+        <v>2</v>
+      </c>
+      <c r="D154">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>52</v>
+      </c>
+      <c r="B155">
+        <v>55</v>
+      </c>
+      <c r="C155">
+        <v>57</v>
+      </c>
+      <c r="D155">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>59</v>
+      </c>
+      <c r="B156">
+        <v>55</v>
+      </c>
+      <c r="C156">
+        <v>33</v>
+      </c>
+      <c r="D156">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>57</v>
+      </c>
+      <c r="B157">
+        <v>56</v>
+      </c>
+      <c r="C157">
+        <v>7</v>
+      </c>
+      <c r="D157">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>58</v>
+      </c>
+      <c r="B158">
+        <v>57</v>
+      </c>
+      <c r="C158">
+        <v>1</v>
+      </c>
+      <c r="D158">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>60</v>
+      </c>
+      <c r="B159">
+        <v>58</v>
+      </c>
+      <c r="C159">
+        <v>49</v>
+      </c>
+      <c r="D159">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>60</v>
+      </c>
+      <c r="B160">
+        <v>59</v>
+      </c>
+      <c r="C160">
+        <v>10</v>
+      </c>
+      <c r="D160">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>60</v>
+      </c>
+      <c r="B161">
+        <v>57</v>
+      </c>
+      <c r="C161">
+        <v>14</v>
+      </c>
+      <c r="D161">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:D124">
-    <sortCondition ref="A41"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:D161">
+    <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>